<commit_message>
Problem Solved Date input to Excel
</commit_message>
<xml_diff>
--- a/Prototype/PHPSCRIPTS/SamanAndrey/ForecastResult2017.xlsx
+++ b/Prototype/PHPSCRIPTS/SamanAndrey/ForecastResult2017.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="6">
   <si>
     <t>ID</t>
   </si>
@@ -33,78 +33,6 @@
   </si>
   <si>
     <t>Upper Confidence Bound</t>
-  </si>
-  <si>
-    <t>2015-01-31</t>
-  </si>
-  <si>
-    <t>2015-02-28</t>
-  </si>
-  <si>
-    <t>2015-03-31</t>
-  </si>
-  <si>
-    <t>2015-04-30</t>
-  </si>
-  <si>
-    <t>2015-05-31</t>
-  </si>
-  <si>
-    <t>2015-06-30</t>
-  </si>
-  <si>
-    <t>2015-07-31</t>
-  </si>
-  <si>
-    <t>2015-08-31</t>
-  </si>
-  <si>
-    <t>2015-09-30</t>
-  </si>
-  <si>
-    <t>2015-10-31</t>
-  </si>
-  <si>
-    <t>2015-11-30</t>
-  </si>
-  <si>
-    <t>2015-12-31</t>
-  </si>
-  <si>
-    <t>2016-01-31</t>
-  </si>
-  <si>
-    <t>2016-02-28</t>
-  </si>
-  <si>
-    <t>2016-03-31</t>
-  </si>
-  <si>
-    <t>2016-04-30</t>
-  </si>
-  <si>
-    <t>2016-05-31</t>
-  </si>
-  <si>
-    <t>2016-06-30</t>
-  </si>
-  <si>
-    <t>2016-07-31</t>
-  </si>
-  <si>
-    <t>2016-08-31</t>
-  </si>
-  <si>
-    <t>2016-09-30</t>
-  </si>
-  <si>
-    <t>2016-10-31</t>
-  </si>
-  <si>
-    <t>2016-11-30</t>
-  </si>
-  <si>
-    <t>2016-12-31</t>
   </si>
 </sst>
 </file>
@@ -449,7 +377,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:G27"/>
+  <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="F10" sqref="F10"/>
@@ -485,217 +413,225 @@
       </c>
     </row>
     <row r="2" spans="1:7">
-      <c r="B2" t="s">
-        <v>6</v>
+      <c r="B2" t="str">
+        <f>DATE(2015,01,31)</f>
+        <v>0</v>
       </c>
       <c r="C2">
         <v>1072</v>
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="B3" t="s">
-        <v>7</v>
+      <c r="B3" t="str">
+        <f>DATE(2015,02,28)</f>
+        <v>0</v>
       </c>
       <c r="C3">
         <v>578</v>
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="B4" t="s">
-        <v>8</v>
+      <c r="B4" t="str">
+        <f>DATE(2015,03,31)</f>
+        <v>0</v>
       </c>
       <c r="C4">
         <v>447</v>
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="B5" t="s">
-        <v>9</v>
+      <c r="B5" t="str">
+        <f>DATE(2015,04,30)</f>
+        <v>0</v>
       </c>
       <c r="C5">
         <v>1074</v>
       </c>
     </row>
     <row r="6" spans="1:7">
-      <c r="B6" t="s">
-        <v>10</v>
+      <c r="B6" t="str">
+        <f>DATE(2015,05,31)</f>
+        <v>0</v>
       </c>
       <c r="C6">
         <v>955</v>
       </c>
     </row>
     <row r="7" spans="1:7">
-      <c r="B7" t="s">
-        <v>11</v>
+      <c r="B7" t="str">
+        <f>DATE(2015,06,30)</f>
+        <v>0</v>
       </c>
       <c r="C7">
         <v>590</v>
       </c>
     </row>
     <row r="8" spans="1:7">
-      <c r="B8" t="s">
-        <v>12</v>
+      <c r="B8" t="str">
+        <f>DATE(2015,07,31)</f>
+        <v>0</v>
       </c>
       <c r="C8">
         <v>467</v>
       </c>
     </row>
     <row r="9" spans="1:7">
-      <c r="B9" t="s">
-        <v>13</v>
+      <c r="B9" t="str">
+        <f>DATE(2015,08,31)</f>
+        <v>0</v>
       </c>
       <c r="C9">
         <v>831</v>
       </c>
     </row>
     <row r="10" spans="1:7">
-      <c r="B10" t="s">
-        <v>14</v>
+      <c r="B10" t="str">
+        <f>DATE(2015,09,30)</f>
+        <v>0</v>
       </c>
       <c r="C10">
         <v>467</v>
       </c>
     </row>
     <row r="11" spans="1:7">
-      <c r="B11" t="s">
-        <v>15</v>
+      <c r="B11" t="str">
+        <f>DATE(2015,10,31)</f>
+        <v>0</v>
       </c>
       <c r="C11">
         <v>636</v>
       </c>
     </row>
     <row r="12" spans="1:7">
-      <c r="B12" t="s">
-        <v>16</v>
+      <c r="B12" t="str">
+        <f>DATE(2015,11,30)</f>
+        <v>0</v>
       </c>
       <c r="C12">
         <v>1088</v>
       </c>
     </row>
     <row r="13" spans="1:7">
-      <c r="B13" t="s">
-        <v>17</v>
+      <c r="B13" t="str">
+        <f>DATE(2015,12,31)</f>
+        <v>0</v>
       </c>
       <c r="C13">
         <v>1402</v>
       </c>
     </row>
     <row r="14" spans="1:7">
-      <c r="B14" t="s">
-        <v>18</v>
+      <c r="B14" t="str">
+        <f>DATE(2016,01,31)</f>
+        <v>0</v>
       </c>
       <c r="C14">
         <v>1072</v>
       </c>
     </row>
     <row r="15" spans="1:7">
-      <c r="B15" t="s">
-        <v>19</v>
+      <c r="B15" t="str">
+        <f>DATE(2016,02,28)</f>
+        <v>0</v>
       </c>
       <c r="C15">
         <v>1186</v>
       </c>
     </row>
     <row r="16" spans="1:7">
-      <c r="B16" t="s">
-        <v>20</v>
+      <c r="B16" t="str">
+        <f>DATE(2016,03,31)</f>
+        <v>0</v>
       </c>
       <c r="C16">
         <v>1268</v>
       </c>
     </row>
     <row r="17" spans="1:7">
-      <c r="B17" t="s">
-        <v>21</v>
+      <c r="B17" t="str">
+        <f>DATE(2016,04,30)</f>
+        <v>0</v>
       </c>
       <c r="C17">
         <v>734</v>
       </c>
     </row>
     <row r="18" spans="1:7">
-      <c r="B18" t="s">
-        <v>22</v>
+      <c r="B18" t="str">
+        <f>DATE(2016,05,31)</f>
+        <v>0</v>
       </c>
       <c r="C18">
         <v>798</v>
       </c>
     </row>
     <row r="19" spans="1:7">
-      <c r="B19" t="s">
-        <v>23</v>
+      <c r="B19" t="str">
+        <f>DATE(2016,06,30)</f>
+        <v>0</v>
       </c>
       <c r="C19">
         <v>791</v>
       </c>
     </row>
     <row r="20" spans="1:7">
-      <c r="B20" t="s">
-        <v>24</v>
+      <c r="B20" t="str">
+        <f>DATE(2016,07,31)</f>
+        <v>0</v>
       </c>
       <c r="C20">
         <v>1100</v>
       </c>
     </row>
     <row r="21" spans="1:7">
-      <c r="B21" t="s">
-        <v>25</v>
+      <c r="B21" t="str">
+        <f>DATE(2016,08,31)</f>
+        <v>0</v>
       </c>
       <c r="C21">
         <v>1003</v>
       </c>
     </row>
     <row r="22" spans="1:7">
-      <c r="B22" t="s">
-        <v>26</v>
+      <c r="B22" t="str">
+        <f>DATE(2016,09,30)</f>
+        <v>0</v>
       </c>
       <c r="C22">
         <v>1223</v>
       </c>
     </row>
     <row r="23" spans="1:7">
-      <c r="B23" t="s">
-        <v>27</v>
+      <c r="B23" t="str">
+        <f>DATE(2016,10,31)</f>
+        <v>0</v>
       </c>
       <c r="C23">
         <v>1440</v>
       </c>
     </row>
     <row r="24" spans="1:7">
-      <c r="B24" t="s">
-        <v>28</v>
+      <c r="B24" t="str">
+        <f>DATE(2016,11,30)</f>
+        <v>0</v>
       </c>
       <c r="C24">
         <v>1161</v>
       </c>
     </row>
     <row r="25" spans="1:7">
-      <c r="B25" t="s">
-        <v>29</v>
+      <c r="B25" t="str">
+        <f>DATE(2016,12,31)</f>
+        <v>0</v>
       </c>
       <c r="C25">
         <v>2686</v>
       </c>
     </row>
     <row r="26" spans="1:7">
-      <c r="D26">
-        <v>45</v>
-      </c>
-      <c r="E26">
-        <v>45</v>
-      </c>
-      <c r="F26">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7">
-      <c r="D27">
-        <v>45</v>
-      </c>
-      <c r="E27">
-        <v>45</v>
-      </c>
-      <c r="F27">
-        <v>45</v>
+      <c r="D26" t="str">
+        <f>FORECAST.ETS(B26,$C$2:$C$25,$B$2:$B$25,1,1)</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>